<commit_message>
Update cell contents to be data jobs focused
</commit_message>
<xml_diff>
--- a/1_Spreadsheets_Intro/1_Worksheets/2_First_Worksheet.xlsx
+++ b/1_Spreadsheets_Intro/1_Worksheets/2_First_Worksheet.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\1_Spreadsheets_Intro\1_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\1_Spreadsheets_Intro\1_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA747150-B93D-47D1-8B70-C329372CAFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086AD7B1-96AF-4BCE-938C-3176F95A0919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="830" yWindow="1660" windowWidth="23810" windowHeight="14980" activeTab="2" xr2:uid="{D15BFCA0-C9DE-46D7-84D4-5CA68B4322C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D15BFCA0-C9DE-46D7-84D4-5CA68B4322C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
-    <sheet name="Final" sheetId="3" r:id="rId2"/>
-    <sheet name="Luke Final" sheetId="4" r:id="rId3"/>
+    <sheet name="Final" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,31 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Shirt</t>
-  </si>
-  <si>
-    <t>Shoes</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Sold Date</t>
-  </si>
-  <si>
-    <t>Total Sales</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Job Title</t>
   </si>
@@ -83,6 +58,9 @@
   </si>
   <si>
     <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Data Engineer</t>
   </si>
 </sst>
 </file>
@@ -134,12 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -148,6 +123,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,16 +464,16 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E4"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,71 +481,67 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2">
-        <v>10</v>
+        <v>70000</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>45479</v>
       </c>
       <c r="E2">
-        <f>B2*C2</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>90000</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>45477</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">B3*C3</f>
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>85000</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>46573</v>
+        <v>45474</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="J4" s="1"/>
+        <v>225</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,148 +549,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F162AAF8-2073-4780-B9E7-D89B3B9F9DBA}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A1:E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45479</v>
-      </c>
-      <c r="E2">
-        <f>B2*C2</f>
-        <v>60</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45477</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">B3*C3</f>
-        <v>140</v>
-      </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52ECFE2-081D-408D-9585-829D17B1B015}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>12</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>70000</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>45479</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5">
-        <v>90000</v>
-      </c>
-      <c r="C3" s="5">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>95000</v>
+      </c>
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>45477</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <v>250</v>
       </c>
     </row>

</xml_diff>